<commit_message>
upload report ver 2
</commit_message>
<xml_diff>
--- a/Docs/Struct Design.xlsx
+++ b/Docs/Struct Design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Network\_Network Game Programming\2017-Network-Game-Programming\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\System32\HomeWork\FinalWOrk\2017-Network-Game-Programming\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>